<commit_message>
Set up OCR to read Data
</commit_message>
<xml_diff>
--- a/EmailPDF/results.xlsx
+++ b/EmailPDF/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cameron Troester\Desktop\EmailPDF\EmailPDF\EmailPDF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Omar Garcia\Documents\Github\EmailPDF\EmailPDF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE17ABD-B941-4028-8186-0EE422619856}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AE676E-EB5F-475D-AC5C-EA550879CCF7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9024" xr2:uid="{86EE2D05-0A1F-4C54-90BD-8153C55DF517}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11430" xr2:uid="{83A4292D-95C2-4BD2-B180-408E4C1DAF61}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -393,14 +391,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{419157DE-3CBF-485D-9EFA-5ACCB18F876D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EAD8EFD-AC4B-4D6D-AC06-E98710514D02}">
   <dimension ref="A2:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>

</xml_diff>